<commit_message>
[Function Managment] Schedule Updated
</commit_message>
<xml_diff>
--- a/PlatformDoc/QPlay/Function Management/Function Managment-Schedule.xlsx
+++ b/PlatformDoc/QPlay/Function Management/Function Managment-Schedule.xlsx
@@ -594,7 +594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -611,48 +611,51 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -677,14 +680,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -999,7 +996,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.85546875" defaultRowHeight="12.75"/>
@@ -1016,18 +1013,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
     </row>
     <row r="2" spans="1:10" ht="24.95" customHeight="1">
       <c r="A2" s="1"/>
@@ -1038,7 +1035,7 @@
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="12" t="s">
         <v>30</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -1058,37 +1055,39 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A3" s="17"/>
-      <c r="B3" s="22" t="s">
+      <c r="A3" s="14"/>
+      <c r="B3" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="15">
         <v>0.25</v>
       </c>
       <c r="F3" s="4">
         <v>1</v>
       </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="7">
+      <c r="G3" s="14"/>
+      <c r="H3" s="6">
         <v>43311</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="6">
         <v>43311</v>
       </c>
-      <c r="J3" s="17"/>
+      <c r="J3" s="6">
+        <v>43311</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A4" s="9">
+      <c r="A4" s="7">
         <v>1</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="9" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="7" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -1101,22 +1100,24 @@
         <v>2</v>
       </c>
       <c r="G4" s="3"/>
-      <c r="H4" s="7">
+      <c r="H4" s="6">
         <v>43311</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="6">
         <v>43311</v>
       </c>
-      <c r="J4" s="8"/>
+      <c r="J4" s="6">
+        <v>43311</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A5" s="9">
+      <c r="A5" s="7">
         <v>2</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="23" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -1129,19 +1130,21 @@
         <v>3</v>
       </c>
       <c r="G5" s="3"/>
-      <c r="H5" s="7">
+      <c r="H5" s="6">
         <v>43311</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="6">
         <v>43311</v>
       </c>
-      <c r="J5" s="8"/>
+      <c r="J5" s="6">
+        <v>43311</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A6" s="9"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="14" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="11" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="2">
@@ -1151,21 +1154,23 @@
         <v>10</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="7">
+      <c r="H6" s="6">
         <v>43321</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="6">
         <v>43321</v>
       </c>
-      <c r="J6" s="8"/>
+      <c r="J6" s="9">
+        <v>43325</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A7" s="9"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="25" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="11" t="s">
         <v>25</v>
       </c>
       <c r="E7" s="2">
@@ -1175,21 +1180,23 @@
         <v>4</v>
       </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <v>43312</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <v>43312</v>
       </c>
-      <c r="J7" s="8"/>
+      <c r="J7" s="6">
+        <v>43312</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A8" s="9">
+      <c r="A8" s="7">
         <v>3</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="14" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="11" t="s">
         <v>23</v>
       </c>
       <c r="E8" s="2">
@@ -1199,23 +1206,25 @@
         <v>5</v>
       </c>
       <c r="G8" s="3"/>
-      <c r="H8" s="7">
+      <c r="H8" s="6">
         <v>43312</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="6">
         <v>43312</v>
       </c>
-      <c r="J8" s="8"/>
+      <c r="J8" s="6">
+        <v>43312</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A9" s="20">
+      <c r="A9" s="21">
         <v>4</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="20" t="s">
+      <c r="B9" s="27"/>
+      <c r="C9" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E9" s="4">
@@ -1224,20 +1233,22 @@
       <c r="F9" s="2">
         <v>6</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="11">
+      <c r="G9" s="8"/>
+      <c r="H9" s="9">
         <v>43313</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="9">
         <v>43313</v>
       </c>
-      <c r="J9" s="12"/>
+      <c r="J9" s="9">
+        <v>43313</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A10" s="21"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="10" t="s">
+      <c r="A10" s="22"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="8" t="s">
         <v>26</v>
       </c>
       <c r="E10" s="4">
@@ -1246,24 +1257,26 @@
       <c r="F10" s="2">
         <v>7</v>
       </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="11">
+      <c r="G10" s="8"/>
+      <c r="H10" s="9">
         <v>43319</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="9">
         <v>43319</v>
       </c>
-      <c r="J10" s="12"/>
+      <c r="J10" s="9">
+        <v>43313</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A11" s="19">
+      <c r="A11" s="20">
         <v>5</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="24" t="s">
+      <c r="B11" s="27"/>
+      <c r="C11" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="8" t="s">
         <v>18</v>
       </c>
       <c r="E11" s="4">
@@ -1273,18 +1286,20 @@
         <v>8</v>
       </c>
       <c r="G11" s="3"/>
-      <c r="H11" s="7">
+      <c r="H11" s="6">
         <v>43320</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="6">
         <v>43320</v>
       </c>
-      <c r="J11" s="8"/>
+      <c r="J11" s="9">
+        <v>43322</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A12" s="19"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="24"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="25"/>
       <c r="D12" s="3" t="s">
         <v>19</v>
       </c>
@@ -1295,18 +1310,20 @@
         <v>9</v>
       </c>
       <c r="G12" s="3"/>
-      <c r="H12" s="7">
+      <c r="H12" s="6">
         <v>43320</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="6">
         <v>43320</v>
       </c>
-      <c r="J12" s="8"/>
+      <c r="J12" s="29">
+        <v>43325</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A13" s="9"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="20" t="s">
+      <c r="A13" s="7"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -1319,19 +1336,21 @@
         <v>11</v>
       </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="7">
+      <c r="H13" s="6">
         <v>43321</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="6">
         <v>43321</v>
       </c>
-      <c r="J13" s="8"/>
+      <c r="J13" s="29">
+        <v>43327</v>
+      </c>
     </row>
     <row r="14" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A14" s="9"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="14" t="s">
+      <c r="A14" s="7"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="11" t="s">
         <v>22</v>
       </c>
       <c r="E14" s="2">
@@ -1341,23 +1360,25 @@
         <v>12</v>
       </c>
       <c r="G14" s="3"/>
-      <c r="H14" s="7">
+      <c r="H14" s="6">
         <v>43321</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14" s="6">
         <v>43325</v>
       </c>
-      <c r="J14" s="8"/>
+      <c r="J14" s="29">
+        <v>43327</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A15" s="13">
+      <c r="A15" s="10">
         <v>8</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="6" t="s">
+      <c r="B15" s="28"/>
+      <c r="C15" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="13" t="s">
         <v>20</v>
       </c>
       <c r="E15" s="4">
@@ -1366,40 +1387,42 @@
       <c r="F15" s="2">
         <v>13</v>
       </c>
-      <c r="G15" s="10"/>
-      <c r="H15" s="7">
+      <c r="G15" s="8"/>
+      <c r="H15" s="6">
         <v>43326</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="6">
         <v>43326</v>
       </c>
-      <c r="J15" s="10"/>
+      <c r="J15" s="29">
+        <v>43327</v>
+      </c>
     </row>
     <row r="16" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A16" s="30"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
     </row>
     <row r="17" spans="1:10" ht="60.75" customHeight="1">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
     </row>
     <row r="18" spans="1:10" ht="24.95" customHeight="1"/>
     <row r="19" spans="1:10" ht="24.95" customHeight="1"/>

</xml_diff>